<commit_message>
fixed plotting blank plots
</commit_message>
<xml_diff>
--- a/Tract 14 WHP Impacts.xlsx
+++ b/Tract 14 WHP Impacts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hilcorp0-my.sharepoint.com/personal/scott_pessetto_hilcorp_com/Documents/code/header_pressure_impact/header_pressure_impact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{9678CAEE-548E-44B3-8760-FFF24A6EFC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31A9D718-6B0F-4B97-AAD0-5D6212FE83C9}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{9678CAEE-548E-44B3-8760-FFF24A6EFC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC1FD9A7-B0A3-40F7-B1D1-3B8B4233A485}"/>
   <bookViews>
-    <workbookView xWindow="39040" yWindow="2050" windowWidth="28800" windowHeight="18050" xr2:uid="{FBFB3C83-6260-49ED-80F1-9A71BB067C5D}"/>
+    <workbookView xWindow="8120" yWindow="2960" windowWidth="28800" windowHeight="15460" xr2:uid="{FBFB3C83-6260-49ED-80F1-9A71BB067C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -265,6 +265,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -567,7 +571,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection sqref="A1:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,7 +652,7 @@
         <v>39.256227346315939</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" ref="I3:I20" si="1">+F3/E3</f>
+        <f>+F3/E3</f>
         <v>10.277321419092647</v>
       </c>
     </row>
@@ -680,7 +684,7 @@
         <v>9.768589725851168</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I3:I20" si="1">+F4/E4</f>
         <v>12.21973323206538</v>
       </c>
     </row>

</xml_diff>